<commit_message>
Finalized schematic, created BOM, started placement (no PCB size yet)
</commit_message>
<xml_diff>
--- a/CONTROLLER_PCB/ESP32 Pinout.xlsx
+++ b/CONTROLLER_PCB/ESP32 Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8055"/>
+    <workbookView windowWidth="20385" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166">
   <si>
     <t>ESP32 pinout</t>
   </si>
@@ -145,18 +145,21 @@
     <t>Camera SIO_D</t>
   </si>
   <si>
+    <t>BOOST_BYPASS</t>
+  </si>
+  <si>
+    <t>IO27</t>
+  </si>
+  <si>
+    <t>A2.7</t>
+  </si>
+  <si>
+    <t>Camera SIO_C</t>
+  </si>
+  <si>
     <t>DATA_OUT</t>
   </si>
   <si>
-    <t>IO27</t>
-  </si>
-  <si>
-    <t>A2.7</t>
-  </si>
-  <si>
-    <t>Camera SIO_C</t>
-  </si>
-  <si>
     <t>IO14</t>
   </si>
   <si>
@@ -388,6 +391,9 @@
     <t>Camera D0 &amp; SD_DATA1 &amp; RGB</t>
   </si>
   <si>
+    <t>LED_GREEN</t>
+  </si>
+  <si>
     <t>IO16</t>
   </si>
   <si>
@@ -424,6 +430,9 @@
     <t>Camera D2 &amp; LCD RST</t>
   </si>
   <si>
+    <t>LED_YELLOW</t>
+  </si>
+  <si>
     <t>IO19</t>
   </si>
   <si>
@@ -431,6 +440,9 @@
   </si>
   <si>
     <t>Camera D3 &amp; LCD CLK</t>
+  </si>
+  <si>
+    <t>LED_RED</t>
   </si>
   <si>
     <t>Tied to pin 37</t>
@@ -507,8 +519,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -528,6 +540,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -536,7 +549,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,24 +563,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -581,15 +586,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -597,7 +603,51 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,47 +669,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -680,49 +692,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,66 +854,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -806,61 +872,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,6 +883,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -898,17 +921,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -928,28 +960,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,29 +983,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -994,130 +1006,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1449,8 +1461,8 @@
   <sheetPr/>
   <dimension ref="B2:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1788,7 +1800,7 @@
         <v>6</v>
       </c>
       <c r="L16" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -1796,34 +1808,34 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
         <v>51</v>
       </c>
-      <c r="H17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" t="s">
-        <v>50</v>
-      </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K17" t="s">
         <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:13">
@@ -1831,37 +1843,37 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" t="s">
         <v>59</v>
       </c>
-      <c r="H18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
       <c r="J18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K18" t="s">
         <v>6</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:12">
@@ -1904,34 +1916,34 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" t="s">
-        <v>66</v>
-      </c>
       <c r="J20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
         <v>6</v>
       </c>
       <c r="L20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:13">
@@ -1939,19 +1951,19 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
@@ -1960,7 +1972,7 @@
         <v>17</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K21" t="s">
         <v>6</v>
@@ -1969,7 +1981,7 @@
         <v>17</v>
       </c>
       <c r="M21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1977,37 +1989,37 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" t="s">
         <v>76</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:13">
@@ -2015,19 +2027,19 @@
         <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>17</v>
@@ -2036,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K23" t="s">
         <v>6</v>
@@ -2045,7 +2057,7 @@
         <v>17</v>
       </c>
       <c r="M23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:13">
@@ -2053,19 +2065,19 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>17</v>
@@ -2074,7 +2086,7 @@
         <v>17</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K24" t="s">
         <v>6</v>
@@ -2083,7 +2095,7 @@
         <v>17</v>
       </c>
       <c r="M24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -2091,19 +2103,19 @@
         <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>17</v>
@@ -2112,7 +2124,7 @@
         <v>17</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K25" t="s">
         <v>6</v>
@@ -2121,7 +2133,7 @@
         <v>17</v>
       </c>
       <c r="M25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:13">
@@ -2129,19 +2141,19 @@
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
@@ -2150,7 +2162,7 @@
         <v>17</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K26" t="s">
         <v>6</v>
@@ -2159,7 +2171,7 @@
         <v>17</v>
       </c>
       <c r="M26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -2167,34 +2179,34 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I27" t="s">
         <v>17</v>
       </c>
       <c r="J27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K27" t="s">
         <v>6</v>
       </c>
       <c r="L27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:13">
@@ -2202,13 +2214,13 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" t="s">
         <v>22</v>
@@ -2217,16 +2229,16 @@
         <v>17</v>
       </c>
       <c r="J28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K28" t="s">
         <v>6</v>
       </c>
       <c r="L28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -2234,31 +2246,31 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K29" t="s">
         <v>6</v>
       </c>
       <c r="L29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="2:12">
@@ -2266,13 +2278,13 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H30" t="s">
         <v>22</v>
@@ -2281,13 +2293,13 @@
         <v>22</v>
       </c>
       <c r="J30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K30" t="s">
         <v>6</v>
       </c>
       <c r="L30" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="2:12">
@@ -2295,16 +2307,16 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H31" t="s">
         <v>22</v>
       </c>
       <c r="I31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J31" t="s">
         <v>22</v>
@@ -2313,7 +2325,7 @@
         <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:12">
@@ -2321,16 +2333,16 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H32" t="s">
         <v>22</v>
       </c>
       <c r="I32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J32" t="s">
         <v>22</v>
@@ -2339,7 +2351,7 @@
         <v>6</v>
       </c>
       <c r="L32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="2:13">
@@ -2347,7 +2359,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H33" t="s">
         <v>22</v>
@@ -2356,16 +2368,16 @@
         <v>22</v>
       </c>
       <c r="J33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K33" t="s">
         <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:12">
@@ -2373,7 +2385,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H34" t="s">
         <v>22</v>
@@ -2382,13 +2394,13 @@
         <v>22</v>
       </c>
       <c r="J34" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K34" t="s">
         <v>6</v>
       </c>
       <c r="L34" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="2:12">
@@ -2396,10 +2408,10 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
@@ -2408,13 +2420,13 @@
         <v>22</v>
       </c>
       <c r="J35" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K35" t="s">
         <v>6</v>
       </c>
       <c r="L35" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="2:12">
@@ -2443,13 +2455,13 @@
         <v>17</v>
       </c>
       <c r="J36" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K36" t="s">
         <v>6</v>
       </c>
       <c r="L36" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="2:12">
@@ -2457,25 +2469,25 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F37" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H37" t="s">
         <v>22</v>
       </c>
       <c r="I37" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="J37" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K37" t="s">
         <v>6</v>
       </c>
       <c r="L37" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="2:13">
@@ -2483,28 +2495,28 @@
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G38" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H38" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="I38" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="J38" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="K38" t="s">
         <v>6</v>
       </c>
       <c r="L38" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M38" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="2:13">
@@ -2512,28 +2524,28 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" t="s">
+        <v>150</v>
+      </c>
+      <c r="I39" t="s">
+        <v>157</v>
+      </c>
+      <c r="J39" t="s">
         <v>152</v>
       </c>
-      <c r="H39" t="s">
-        <v>146</v>
-      </c>
-      <c r="I39" t="s">
-        <v>153</v>
-      </c>
-      <c r="J39" t="s">
-        <v>148</v>
-      </c>
       <c r="K39" t="s">
         <v>6</v>
       </c>
       <c r="L39" t="s">
+        <v>158</v>
+      </c>
+      <c r="M39" t="s">
         <v>154</v>
-      </c>
-      <c r="M39" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="40" spans="2:12">
@@ -2541,28 +2553,28 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F40" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G40" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H40" t="s">
         <v>22</v>
       </c>
       <c r="I40" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="J40" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="K40" t="s">
         <v>6</v>
       </c>
       <c r="L40" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="2:12">
@@ -2570,7 +2582,7 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H41" t="s">
         <v>22</v>
@@ -2579,13 +2591,13 @@
         <v>22</v>
       </c>
       <c r="J41" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="K41" t="s">
         <v>6</v>
       </c>
       <c r="L41" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="2:12">

</xml_diff>